<commit_message>
Get broader range for N.
</commit_message>
<xml_diff>
--- a/RegularityCondition.xlsx
+++ b/RegularityCondition.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="37920" windowHeight="22960" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="39900" windowHeight="26420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -353,10 +353,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G26"/>
+  <dimension ref="B2:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="196" zoomScaleNormal="196" zoomScalePageLayoutView="196" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D26"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -375,7 +375,7 @@
         <v>3</v>
       </c>
       <c r="G2">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
@@ -393,301 +393,114 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4">
-        <v>2</v>
+        <f>B3*10</f>
+        <v>10</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C26" si="0">LOG(B4,2)</f>
-        <v>1</v>
+        <f t="shared" ref="C4:C11" si="0">LOG(B4,2)</f>
+        <v>3.3219280948873626</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D26" si="1">POWER(B4,$G$2)</f>
-        <v>1.4142135623730951</v>
+        <f t="shared" ref="D4:D11" si="1">POWER(B4,$G$2)</f>
+        <v>1.778279410038923</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5">
-        <v>3</v>
+        <f t="shared" ref="B5:B12" si="2">B4*10</f>
+        <v>100</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>1.5849625007211563</v>
+        <v>6.6438561897747253</v>
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
-        <v>1.7320508075688772</v>
+        <v>3.1622776601683795</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6">
-        <v>4</v>
+        <f t="shared" si="2"/>
+        <v>1000</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>9.965784284662087</v>
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>5.6234132519034903</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7">
-        <v>5</v>
+        <f t="shared" si="2"/>
+        <v>10000</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>2.3219280948873622</v>
+        <v>13.287712379549451</v>
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
-        <v>2.2360679774997898</v>
+        <v>10.000000000000002</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B8">
-        <v>6</v>
+        <f t="shared" si="2"/>
+        <v>100000</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>2.5849625007211561</v>
+        <v>16.609640474436812</v>
       </c>
       <c r="D8">
         <f t="shared" si="1"/>
-        <v>2.4494897427831779</v>
+        <v>17.782794100389228</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9">
-        <v>7</v>
+        <f t="shared" si="2"/>
+        <v>1000000</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>2.8073549220576042</v>
+        <v>19.931568569324174</v>
       </c>
       <c r="D9">
         <f t="shared" si="1"/>
-        <v>2.6457513110645907</v>
+        <v>31.622776601683789</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10">
-        <v>8</v>
+        <f t="shared" si="2"/>
+        <v>10000000</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>23.253496664211539</v>
       </c>
       <c r="D10">
         <f t="shared" si="1"/>
-        <v>2.8284271247461903</v>
+        <v>56.234132519034915</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11">
-        <v>9</v>
+        <f t="shared" si="2"/>
+        <v>100000000</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>3.1699250014423126</v>
+        <v>26.575424759098901</v>
       </c>
       <c r="D11">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12">
-        <v>10</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="0"/>
-        <v>3.3219280948873626</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="1"/>
-        <v>3.1622776601683795</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B13">
-        <v>11</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="0"/>
-        <v>3.4594316186372978</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="1"/>
-        <v>3.3166247903553998</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14">
-        <v>12</v>
-      </c>
-      <c r="C14">
-        <f t="shared" si="0"/>
-        <v>3.5849625007211565</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="1"/>
-        <v>3.4641016151377544</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15">
-        <v>13</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="0"/>
-        <v>3.7004397181410922</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="1"/>
-        <v>3.6055512754639891</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B16">
-        <v>14</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="0"/>
-        <v>3.8073549220576037</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="1"/>
-        <v>3.7416573867739413</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B17">
-        <v>15</v>
-      </c>
-      <c r="C17">
-        <f t="shared" si="0"/>
-        <v>3.9068905956085187</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="1"/>
-        <v>3.872983346207417</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18">
-        <v>16</v>
-      </c>
-      <c r="C18">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B19">
-        <v>17</v>
-      </c>
-      <c r="C19">
-        <f>LOG(B19,2)</f>
-        <v>4.08746284125034</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="1"/>
-        <v>4.1231056256176606</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B20">
-        <v>18</v>
-      </c>
-      <c r="C20">
-        <f t="shared" si="0"/>
-        <v>4.1699250014423122</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="1"/>
-        <v>4.2426406871192848</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21">
-        <v>19</v>
-      </c>
-      <c r="C21">
-        <f t="shared" si="0"/>
-        <v>4.2479275134435852</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="1"/>
-        <v>4.358898943540674</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22">
-        <v>20</v>
-      </c>
-      <c r="C22">
-        <f t="shared" si="0"/>
-        <v>4.3219280948873626</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="1"/>
-        <v>4.4721359549995796</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B23">
-        <v>21</v>
-      </c>
-      <c r="C23">
-        <f t="shared" si="0"/>
-        <v>4.3923174227787607</v>
-      </c>
-      <c r="D23">
-        <f t="shared" si="1"/>
-        <v>4.5825756949558398</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24">
-        <v>22</v>
-      </c>
-      <c r="C24">
-        <f t="shared" si="0"/>
-        <v>4.4594316186372973</v>
-      </c>
-      <c r="D24">
-        <f t="shared" si="1"/>
-        <v>4.6904157598234297</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B25">
-        <v>23</v>
-      </c>
-      <c r="C25">
-        <f t="shared" si="0"/>
-        <v>4.5235619560570131</v>
-      </c>
-      <c r="D25">
-        <f t="shared" si="1"/>
-        <v>4.7958315233127191</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B26">
-        <v>24</v>
-      </c>
-      <c r="C26">
-        <f t="shared" si="0"/>
-        <v>4.584962500721157</v>
-      </c>
-      <c r="D26">
-        <f t="shared" si="1"/>
-        <v>4.8989794855663558</v>
+        <v>100.00000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>